<commit_message>
Added new about page, more columns, download function, more studies. This is the 'launch' version
</commit_message>
<xml_diff>
--- a/Data/List_of_studies.xlsx
+++ b/Data/List_of_studies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelberry/Documents/Rescape/Shiny_app/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963D3A75-7DA7-494F-8C41-5D9D31471081}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{99FD11BC-4CFD-1647-B0B4-6B46D5DCDC06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="207">
   <si>
     <t>Title</t>
   </si>
@@ -639,6 +639,18 @@
   </si>
   <si>
     <t>Biofeedback, Anxiety/ Stress, Methods Development</t>
+  </si>
+  <si>
+    <t>The Impact of Virtual Reality on Chronic Pain</t>
+  </si>
+  <si>
+    <t>PloS One</t>
+  </si>
+  <si>
+    <t>Jones, Ted; Moore, Todd; Choo, James</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1371/journal.pone.0167523</t>
   </si>
 </sst>
 </file>
@@ -1492,8 +1504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2784,9 +2796,33 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>203</v>
+      </c>
+      <c r="B41">
+        <v>2016</v>
+      </c>
+      <c r="C41" t="s">
+        <v>204</v>
+      </c>
+      <c r="D41" t="s">
+        <v>205</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F41" t="s">
+        <v>177</v>
+      </c>
+      <c r="G41" t="s">
+        <v>136</v>
+      </c>
+      <c r="K41" t="s">
+        <v>131</v>
+      </c>
       <c r="L41" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    </v>
+        <v xml:space="preserve">Pain Patient Study   </v>
       </c>
     </row>
   </sheetData>
@@ -2830,6 +2866,7 @@
     <hyperlink ref="E36" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
     <hyperlink ref="E37" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
     <hyperlink ref="E38" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="E41" r:id="rId40" xr:uid="{A479E85E-8CC1-8E4C-8053-251EACA44299}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>